<commit_message>
Updated statistics for track 3.
</commit_message>
<xml_diff>
--- a/review/statistics/statistics.xlsx
+++ b/review/statistics/statistics.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mqbprmr4/Projects/mxv/review/statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{65D9AC38-3524-EC48-8D1A-ED03027F262E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19260"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Track 2" sheetId="1" r:id="rId1"/>
+    <sheet name="Track 3" sheetId="2" r:id="rId1"/>
+    <sheet name="Track 2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Amendments</t>
   </si>
@@ -54,13 +56,20 @@
   </si>
   <si>
     <t>Total members</t>
+  </si>
+  <si>
+    <t>[voting not open yet]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,6 +80,13 @@
     <font>
       <b/>
       <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,14 +111,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,17 +433,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0F67A2-B0A4-D848-AAF3-91B26239A724}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -442,69 +462,185 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>51</v>
-      </c>
-      <c r="C2">
-        <v>39</v>
+      <c r="B2" s="2">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>291</v>
-      </c>
-      <c r="C3">
-        <v>166</v>
+      <c r="B3" s="2">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>116</v>
-      </c>
-      <c r="C4">
-        <v>82</v>
+      <c r="B4" s="2">
+        <v>48</v>
+      </c>
+      <c r="C4" s="2">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>958</v>
-      </c>
-      <c r="C5">
-        <v>626</v>
-      </c>
+      <c r="B5" s="2">
+        <v>375</v>
+      </c>
+      <c r="C5" s="2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>38237</v>
-      </c>
+      <c r="B7" s="2">
+        <v>38824</v>
+      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>8373</v>
-      </c>
+      <c r="B8" s="2">
+        <v>8558</v>
+      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>291</v>
+      </c>
+      <c r="C3" s="2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>116</v>
+      </c>
+      <c r="C4" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>958</v>
+      </c>
+      <c r="C5" s="2">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>38237</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>8373</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
         <v>3829</v>
       </c>
+      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>